<commit_message>
updated code for inputting test data from excel
Modified test scripts for feeding the test data from excel
</commit_message>
<xml_diff>
--- a/src/test/java/Data/TestData.xlsx
+++ b/src/test/java/Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhin\eclipse-workspace\PlanitAssesment\src\test\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EBC149-F645-4C31-9C22-CFF526892A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837D6A31-C6F3-4152-8F5E-37638FA3DFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,35 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>CaseType</t>
   </si>
   <si>
-    <t>LoginID</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>abcdef</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>abcdeh</t>
-  </si>
-  <si>
-    <t>123457</t>
-  </si>
-  <si>
-    <t>abcdeb</t>
-  </si>
-  <si>
-    <t>123458</t>
-  </si>
-  <si>
     <t>TestCase1</t>
   </si>
   <si>
@@ -61,13 +37,67 @@
   </si>
   <si>
     <t>TestCase3</t>
+  </si>
+  <si>
+    <t>ForeName_ExpectedErrMessage</t>
+  </si>
+  <si>
+    <t>Email_ExpectedErrMessage</t>
+  </si>
+  <si>
+    <t>Message_ExpectedErrMessage</t>
+  </si>
+  <si>
+    <t>Forename is required</t>
+  </si>
+  <si>
+    <t>Email is required</t>
+  </si>
+  <si>
+    <t>Message is required</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>ForeName</t>
+  </si>
+  <si>
+    <t>Abhinav</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Abhinav.agrawal88@gmail.com</t>
+  </si>
+  <si>
+    <t>input message for testcase 1</t>
+  </si>
+  <si>
+    <t>StuffedFrogQuantity</t>
+  </si>
+  <si>
+    <t>FluffyBunnyQuantity</t>
+  </si>
+  <si>
+    <t>ValentineBearQuantity</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +107,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,14 +137,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,63 +427,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="1"/>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
+      <c r="C4" s="1"/>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{A74EA29B-CE7D-4527-B0EA-DBA04AC914C4}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{4B8DD662-55A4-4127-AAC1-40AA1E17D991}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>